<commit_message>
refactoring - Daily chart correction. This is final Commercial version
</commit_message>
<xml_diff>
--- a/Total_Stat.xlsx
+++ b/Total_Stat.xlsx
@@ -287,9 +287,12 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Daily!$A$1</c:f>
+              <c:f>Daily!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Анатолий</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -298,9 +301,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Daily!$A$2:$A$12</c:f>
+              <c:f>Daily!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>03.01.2023</c:v>
                 </c:pt>
@@ -336,39 +339,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Daily!$A$2:$A$12</c:f>
+              <c:f>Daily!$B$2:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>482</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>476</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>511</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -379,11 +361,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Daily!$B$1</c:f>
+              <c:f>Daily!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Анатолий</c:v>
+                  <c:v>Антон</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -393,9 +375,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Daily!$A$2:$A$12</c:f>
+              <c:f>Daily!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>03.01.2023</c:v>
                 </c:pt>
@@ -431,18 +413,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Daily!$B$2:$B$12</c:f>
+              <c:f>Daily!$C$2:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>482</c:v>
-                </c:pt>
+                <c:ptCount val="10"/>
                 <c:pt idx="3">
-                  <c:v>476</c:v>
+                  <c:v>475</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>511</c:v>
+                  <c:v>434</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>396</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -453,11 +435,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Daily!$C$1</c:f>
+              <c:f>Daily!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Антон</c:v>
+                  <c:v>Антон Б</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -467,9 +449,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Daily!$A$2:$A$12</c:f>
+              <c:f>Daily!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>03.01.2023</c:v>
                 </c:pt>
@@ -505,18 +487,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Daily!$C$2:$C$12</c:f>
+              <c:f>Daily!$D$2:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="3">
-                  <c:v>475</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>434</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>396</c:v>
+                <c:ptCount val="10"/>
+                <c:pt idx="1">
+                  <c:v>452</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -527,11 +503,11 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Daily!$D$1</c:f>
+              <c:f>Daily!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Антон Б</c:v>
+                  <c:v>Вася</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -541,9 +517,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Daily!$A$2:$A$12</c:f>
+              <c:f>Daily!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>03.01.2023</c:v>
                 </c:pt>
@@ -579,12 +555,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Daily!$D$2:$D$12</c:f>
+              <c:f>Daily!$E$2:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="1">
-                  <c:v>452</c:v>
+                <c:ptCount val="10"/>
+                <c:pt idx="6">
+                  <c:v>460</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -595,11 +571,11 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Daily!$E$1</c:f>
+              <c:f>Daily!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Вася</c:v>
+                  <c:v>Гоша</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -609,9 +585,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Daily!$A$2:$A$12</c:f>
+              <c:f>Daily!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>03.01.2023</c:v>
                 </c:pt>
@@ -647,12 +623,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Daily!$E$2:$E$12</c:f>
+              <c:f>Daily!$F$2:$F$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>504</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>463</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>573</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>581</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>543</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>569</c:v>
+                </c:pt>
                 <c:pt idx="6">
-                  <c:v>460</c:v>
+                  <c:v>593</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -663,11 +657,11 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Daily!$F$1</c:f>
+              <c:f>Daily!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Гоша</c:v>
+                  <c:v>Денис</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -677,9 +671,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Daily!$A$2:$A$12</c:f>
+              <c:f>Daily!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>03.01.2023</c:v>
                 </c:pt>
@@ -715,30 +709,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Daily!$F$2:$F$12</c:f>
+              <c:f>Daily!$G$2:$G$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>504</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>463</c:v>
-                </c:pt>
+                <c:ptCount val="10"/>
                 <c:pt idx="2">
-                  <c:v>573</c:v>
+                  <c:v>518</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>581</c:v>
+                  <c:v>516</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>466</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>543</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>569</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>593</c:v>
+                  <c:v>565</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>516</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -749,11 +740,11 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Daily!$G$1</c:f>
+              <c:f>Daily!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Денис</c:v>
+                  <c:v>Дима К</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -763,9 +754,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Daily!$A$2:$A$12</c:f>
+              <c:f>Daily!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>03.01.2023</c:v>
                 </c:pt>
@@ -801,27 +792,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Daily!$G$2:$G$12</c:f>
+              <c:f>Daily!$H$2:$H$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="2">
-                  <c:v>518</c:v>
-                </c:pt>
+                <c:ptCount val="10"/>
                 <c:pt idx="3">
-                  <c:v>516</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>466</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>543</c:v>
+                  <c:v>476</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>565</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>516</c:v>
+                  <c:v>492</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>506</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -832,11 +817,11 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Daily!$H$1</c:f>
+              <c:f>Daily!$I$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Дима К</c:v>
+                  <c:v>Дима Н</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -846,9 +831,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Daily!$A$2:$A$12</c:f>
+              <c:f>Daily!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>03.01.2023</c:v>
                 </c:pt>
@@ -884,21 +869,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Daily!$H$2:$H$12</c:f>
+              <c:f>Daily!$I$2:$I$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>554</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>566</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>486</c:v>
+                </c:pt>
                 <c:pt idx="3">
-                  <c:v>476</c:v>
+                  <c:v>556</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>574</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>571</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>492</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>510</c:v>
+                  <c:v>556</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>503</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>506</c:v>
+                  <c:v>511</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -909,11 +909,11 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>Daily!$I$1</c:f>
+              <c:f>Daily!$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Дима Н</c:v>
+                  <c:v>Дима С</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -923,9 +923,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Daily!$A$2:$A$12</c:f>
+              <c:f>Daily!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>03.01.2023</c:v>
                 </c:pt>
@@ -961,36 +961,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Daily!$I$2:$I$12</c:f>
+              <c:f>Daily!$J$2:$J$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>554</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>566</c:v>
-                </c:pt>
+                <c:ptCount val="10"/>
                 <c:pt idx="2">
-                  <c:v>486</c:v>
+                  <c:v>466</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>556</c:v>
+                  <c:v>519</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>574</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>571</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>556</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>503</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>511</c:v>
+                  <c:v>525</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1001,11 +983,11 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>Daily!$J$1</c:f>
+              <c:f>Daily!$K$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Дима С</c:v>
+                  <c:v>Женя</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1015,9 +997,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Daily!$A$2:$A$12</c:f>
+              <c:f>Daily!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>03.01.2023</c:v>
                 </c:pt>
@@ -1053,18 +1035,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Daily!$J$2:$J$12</c:f>
+              <c:f>Daily!$K$2:$K$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="2">
-                  <c:v>466</c:v>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>534</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>549</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>519</c:v>
+                  <c:v>470</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>525</c:v>
+                  <c:v>515</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>501</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>547</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>595</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1075,11 +1069,11 @@
           <c:order val="10"/>
           <c:tx>
             <c:strRef>
-              <c:f>Daily!$K$1</c:f>
+              <c:f>Daily!$L$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Женя</c:v>
+                  <c:v>Ира</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1089,9 +1083,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Daily!$A$2:$A$12</c:f>
+              <c:f>Daily!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>03.01.2023</c:v>
                 </c:pt>
@@ -1127,30 +1121,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Daily!$K$2:$K$12</c:f>
+              <c:f>Daily!$L$2:$L$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>534</c:v>
-                </c:pt>
+                <c:ptCount val="10"/>
                 <c:pt idx="1">
-                  <c:v>549</c:v>
+                  <c:v>437</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>470</c:v>
+                  <c:v>454</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>515</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>501</c:v>
+                  <c:v>418</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>359</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>547</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>595</c:v>
+                  <c:v>337</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1161,11 +1149,11 @@
           <c:order val="11"/>
           <c:tx>
             <c:strRef>
-              <c:f>Daily!$L$1</c:f>
+              <c:f>Daily!$M$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ира</c:v>
+                  <c:v>Коля</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1175,9 +1163,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Daily!$A$2:$A$12</c:f>
+              <c:f>Daily!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>03.01.2023</c:v>
                 </c:pt>
@@ -1213,24 +1201,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Daily!$L$2:$L$12</c:f>
+              <c:f>Daily!$M$2:$M$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>514</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>437</c:v>
+                  <c:v>541</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>542</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>454</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>418</c:v>
+                  <c:v>583</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>359</c:v>
+                  <c:v>572</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>337</c:v>
+                  <c:v>531</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>508</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1241,11 +1235,11 @@
           <c:order val="12"/>
           <c:tx>
             <c:strRef>
-              <c:f>Daily!$M$1</c:f>
+              <c:f>Daily!$N$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Коля</c:v>
+                  <c:v>Ксения</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1255,9 +1249,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Daily!$A$2:$A$12</c:f>
+              <c:f>Daily!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>03.01.2023</c:v>
                 </c:pt>
@@ -1293,30 +1287,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Daily!$M$2:$M$12</c:f>
+              <c:f>Daily!$N$2:$N$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>514</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>541</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>542</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>583</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>572</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>531</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>508</c:v>
+                <c:ptCount val="10"/>
+                <c:pt idx="4">
+                  <c:v>488</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1327,11 +1303,11 @@
           <c:order val="13"/>
           <c:tx>
             <c:strRef>
-              <c:f>Daily!$N$1</c:f>
+              <c:f>Daily!$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ксения</c:v>
+                  <c:v>Леша</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1341,9 +1317,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Daily!$A$2:$A$12</c:f>
+              <c:f>Daily!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>03.01.2023</c:v>
                 </c:pt>
@@ -1379,12 +1355,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Daily!$N$2:$N$12</c:f>
+              <c:f>Daily!$O$2:$O$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="4">
-                  <c:v>488</c:v>
+                <c:ptCount val="10"/>
+                <c:pt idx="3">
+                  <c:v>481</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>493</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1395,11 +1374,11 @@
           <c:order val="14"/>
           <c:tx>
             <c:strRef>
-              <c:f>Daily!$O$1</c:f>
+              <c:f>Daily!$P$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Леша</c:v>
+                  <c:v>Макс</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1409,9 +1388,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Daily!$A$2:$A$12</c:f>
+              <c:f>Daily!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>03.01.2023</c:v>
                 </c:pt>
@@ -1447,15 +1426,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Daily!$O$2:$O$12</c:f>
+              <c:f>Daily!$P$2:$P$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>412</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>468</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>466</c:v>
+                </c:pt>
                 <c:pt idx="3">
-                  <c:v>481</c:v>
+                  <c:v>527</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>514</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>549</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>493</c:v>
+                  <c:v>483</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1466,11 +1463,11 @@
           <c:order val="15"/>
           <c:tx>
             <c:strRef>
-              <c:f>Daily!$P$1</c:f>
+              <c:f>Daily!$Q$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Макс</c:v>
+                  <c:v>Миша</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1480,9 +1477,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Daily!$A$2:$A$12</c:f>
+              <c:f>Daily!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>03.01.2023</c:v>
                 </c:pt>
@@ -1518,33 +1515,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Daily!$P$2:$P$12</c:f>
+              <c:f>Daily!$Q$2:$Q$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>412</c:v>
-                </c:pt>
+                <c:ptCount val="10"/>
                 <c:pt idx="1">
-                  <c:v>468</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>466</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>527</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>480</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>514</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>549</c:v>
+                  <c:v>492</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>487</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>437</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>483</c:v>
+                  <c:v>456</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1555,11 +1540,11 @@
           <c:order val="16"/>
           <c:tx>
             <c:strRef>
-              <c:f>Daily!$Q$1</c:f>
+              <c:f>Daily!$R$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Миша</c:v>
+                  <c:v>Ольга</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1569,9 +1554,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Daily!$A$2:$A$12</c:f>
+              <c:f>Daily!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>03.01.2023</c:v>
                 </c:pt>
@@ -1607,21 +1592,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Daily!$Q$2:$Q$12</c:f>
+              <c:f>Daily!$R$2:$R$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="1">
-                  <c:v>492</c:v>
-                </c:pt>
+                <c:ptCount val="10"/>
                 <c:pt idx="4">
-                  <c:v>487</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>437</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>456</c:v>
+                  <c:v>427</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1632,11 +1608,11 @@
           <c:order val="17"/>
           <c:tx>
             <c:strRef>
-              <c:f>Daily!$R$1</c:f>
+              <c:f>Daily!$S$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ольга</c:v>
+                  <c:v>Паша</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1646,9 +1622,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Daily!$A$2:$A$12</c:f>
+              <c:f>Daily!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>03.01.2023</c:v>
                 </c:pt>
@@ -1684,12 +1660,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Daily!$R$2:$R$12</c:f>
+              <c:f>Daily!$S$2:$S$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
+                <c:pt idx="3">
+                  <c:v>484</c:v>
+                </c:pt>
                 <c:pt idx="4">
-                  <c:v>427</c:v>
+                  <c:v>526</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>565</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>605</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>605</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1700,11 +1688,11 @@
           <c:order val="18"/>
           <c:tx>
             <c:strRef>
-              <c:f>Daily!$S$1</c:f>
+              <c:f>Daily!$T$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Паша</c:v>
+                  <c:v>Рома А</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1714,9 +1702,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Daily!$A$2:$A$12</c:f>
+              <c:f>Daily!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>03.01.2023</c:v>
                 </c:pt>
@@ -1752,24 +1740,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Daily!$S$2:$S$12</c:f>
+              <c:f>Daily!$T$2:$T$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
+                <c:pt idx="2">
+                  <c:v>478</c:v>
+                </c:pt>
                 <c:pt idx="3">
                   <c:v>484</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>526</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>565</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>605</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>605</c:v>
+                  <c:v>542</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>584</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1780,11 +1765,11 @@
           <c:order val="19"/>
           <c:tx>
             <c:strRef>
-              <c:f>Daily!$T$1</c:f>
+              <c:f>Daily!$U$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Рома А</c:v>
+                  <c:v>Рома К</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1794,9 +1779,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Daily!$A$2:$A$12</c:f>
+              <c:f>Daily!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>03.01.2023</c:v>
                 </c:pt>
@@ -1832,21 +1817,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Daily!$T$2:$T$12</c:f>
+              <c:f>Daily!$U$2:$U$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="2">
-                  <c:v>478</c:v>
-                </c:pt>
+                <c:ptCount val="10"/>
                 <c:pt idx="3">
-                  <c:v>484</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>542</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>584</c:v>
+                  <c:v>502</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1857,11 +1833,11 @@
           <c:order val="20"/>
           <c:tx>
             <c:strRef>
-              <c:f>Daily!$U$1</c:f>
+              <c:f>Daily!$V$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Рома К</c:v>
+                  <c:v>Саша</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1871,9 +1847,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Daily!$A$2:$A$12</c:f>
+              <c:f>Daily!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>03.01.2023</c:v>
                 </c:pt>
@@ -1909,12 +1885,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Daily!$U$2:$U$12</c:f>
+              <c:f>Daily!$V$2:$V$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="3">
-                  <c:v>502</c:v>
+                <c:ptCount val="10"/>
+                <c:pt idx="4">
+                  <c:v>494</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>583</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>565</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1925,11 +1907,11 @@
           <c:order val="21"/>
           <c:tx>
             <c:strRef>
-              <c:f>Daily!$V$1</c:f>
+              <c:f>Daily!$W$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Саша</c:v>
+                  <c:v>Сергей</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1939,9 +1921,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Daily!$A$2:$A$12</c:f>
+              <c:f>Daily!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>03.01.2023</c:v>
                 </c:pt>
@@ -1977,18 +1959,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Daily!$V$2:$V$12</c:f>
+              <c:f>Daily!$W$2:$W$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="4">
-                  <c:v>494</c:v>
+                <c:ptCount val="10"/>
+                <c:pt idx="3">
+                  <c:v>506</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>583</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>565</c:v>
+                  <c:v>441</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1999,11 +1978,11 @@
           <c:order val="22"/>
           <c:tx>
             <c:strRef>
-              <c:f>Daily!$W$1</c:f>
+              <c:f>Daily!$X$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Сергей</c:v>
+                  <c:v>Соня</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2013,9 +1992,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Daily!$A$2:$A$12</c:f>
+              <c:f>Daily!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>03.01.2023</c:v>
                 </c:pt>
@@ -2051,15 +2030,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Daily!$W$2:$W$12</c:f>
+              <c:f>Daily!$X$2:$X$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="3">
-                  <c:v>506</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>441</c:v>
+                  <c:v>392</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2070,11 +2046,11 @@
           <c:order val="23"/>
           <c:tx>
             <c:strRef>
-              <c:f>Daily!$X$1</c:f>
+              <c:f>Daily!$Y$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Соня</c:v>
+                  <c:v>Таня</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2084,9 +2060,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Daily!$A$2:$A$12</c:f>
+              <c:f>Daily!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>03.01.2023</c:v>
                 </c:pt>
@@ -2122,12 +2098,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Daily!$X$2:$X$12</c:f>
+              <c:f>Daily!$Y$2:$Y$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
+                <c:pt idx="2">
+                  <c:v>551</c:v>
+                </c:pt>
                 <c:pt idx="3">
-                  <c:v>392</c:v>
+                  <c:v>563</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>569</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>561</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>569</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2138,11 +2126,11 @@
           <c:order val="24"/>
           <c:tx>
             <c:strRef>
-              <c:f>Daily!$Y$1</c:f>
+              <c:f>Daily!$Z$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Таня</c:v>
+                  <c:v>Толик</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2152,9 +2140,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Daily!$A$2:$A$12</c:f>
+              <c:f>Daily!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>03.01.2023</c:v>
                 </c:pt>
@@ -2190,24 +2178,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Daily!$Y$2:$Y$12</c:f>
+              <c:f>Daily!$Z$2:$Z$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
+                <c:pt idx="1">
+                  <c:v>546</c:v>
+                </c:pt>
                 <c:pt idx="2">
-                  <c:v>551</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>563</c:v>
+                  <c:v>502</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>550</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>569</c:v>
+                  <c:v>518</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>561</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>569</c:v>
+                  <c:v>573</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>

</xml_diff>

<commit_message>
refactoring - Total chart correction. Make color better.
</commit_message>
<xml_diff>
--- a/Total_Stat.xlsx
+++ b/Total_Stat.xlsx
@@ -183,7 +183,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[Green]General;[Red]-General;General"/>
+    <numFmt numFmtId="164" formatCode="[Blue]General;[Red]-General;General"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -210,7 +210,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -219,7 +219,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
+        <fgColor rgb="FFDEDEDE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE4E4E4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -262,7 +268,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>